<commit_message>
writes ng-click to console log tile number
</commit_message>
<xml_diff>
--- a/resources/pixel world.xlsx
+++ b/resources/pixel world.xlsx
@@ -30,10 +30,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -62,15 +78,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -372,8 +392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AP25" sqref="AP25"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AZ34" sqref="AZ34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4098,7 +4118,12 @@
     <row r="30" spans="1:61" s="2" customFormat="1"/>
     <row r="31" spans="1:61" s="2" customFormat="1"/>
     <row r="32" spans="1:61" s="2" customFormat="1"/>
-    <row r="33" s="2" customFormat="1"/>
+    <row r="33" spans="52:52" s="2" customFormat="1">
+      <c r="AZ33" s="2" t="str">
+        <f>CONCATENATE("[", AZ1, ",",AZ2, ",",AZ3, ",",AZ4, ",",AZ5, ",",AZ6, ",",AZ7, ",",AZ8, ",",AZ9, ",",AZ10, ",",AZ11, ",",AZ12, ",",AZ13, ",",AZ14, ",",AZ15, ",",AZ16, ",",AZ17, ",",AZ18, ",",AZ19, ",",AZ20, ",",AZ21, ",",AZ22, ",",AZ23, "]")</f>
+        <v>[[0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,0,0,0,0,0,0,0,0,0,0,0,0,0],[0,0,0,0,0,0,0,0,0,0,0,1,1,1,0,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,0,0,0,0,0,0,0,0,0,0,0],[0,0,0,0,0,0,0,0,0,0,0,1,0,0,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0],[0,0,0,0,0,0,0,1,1,1,0,0,1,1,0,0,1,1,1,0,0,0,0,0,0,0,0,1,1,0,0,0,0,1,1,1,1,1,1,1,1,1,1,1,1,1,0,0,0,0],[0,0,1,1,1,1,1,1,1,1,1,1,0,1,1,0,0,1,1,0,0,0,0,0,0,0,1,1,1,1,0,0,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,0,0],[0,0,1,1,1,1,1,1,1,1,1,1,0,0,0,0,0,1,0,0,0,0,0,0,0,0,1,1,0,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,0],[0,1,0,0,0,1,1,1,1,1,1,0,0,1,1,0,0,0,0,0,0,0,0,0,1,0,0,0,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,0,1,0,0,0],[0,0,0,0,0,1,1,1,1,1,1,1,0,1,1,1,0,0,0,0,0,0,0,0,0,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,0,0,1,0,0,0],[0,0,0,0,0,0,1,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,0,0,1,0,0,0,0],[0,0,0,0,0,0,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,1,1,0,1,0,1,0,0,1,1,1,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0],[0,0,0,0,0,0,0,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,0,1,1,1,1,1,1,1,1,1,1,1,1,0,0,1,0,0,0,0,0,0],[0,0,0,0,0,0,0,0,1,1,0,0,1,0,0,0,0,0,0,0,0,0,0,1,1,1,0,0,0,1,1,0,1,1,1,1,1,1,1,1,1,0,1,0,0,0,0,0,0,0],[0,0,0,0,0,0,0,0,0,1,1,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,1,1,1,0,1,1,0,0,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0],[0,0,0,0,0,0,0,0,0,0,1,1,0,0,0,0,0,0,0,0,0,0,1,1,1,1,1,1,1,0,0,0,0,0,1,1,0,0,1,1,0,1,0,0,0,0,0,0,0,0],[0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,0,0,0,0,0,0,0,1,1,1,1,1,1,1,1,1,0,0,0,0,1,0,0,1,0,0,0,0,0,0,0,0,0,0,0],[0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,1,0,0,0,0,0,0,0,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,1,1,0,0,0,0,0,0,0,0,0],[0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,1,1,1,0,0,0,0,0,0,0,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0],[0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,1,0,0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,1,0,1,0,0,0,0,0,0,0],[0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,1,1,1,0,0,0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0],[0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,0,0,0,0,0,0,0,0,0,0,1,1,1,0,0,0,0,0,0,0,0,0,1,1,1,1,1,1,0,0,0,0,0,0],[0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,0,0,0,0,0,0,0,0,0,0,0,0,1,0,0,0,0,0,0,0,0,0,0,1,1,1,1,1,1,0,0,0,0,0,0],[0,0,0,0,0,0,0,0,0,0,0,0,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,0,0,0,0,0,0,0],[0,0,0,0,0,0,0,0,0,0,0,0,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0]]</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AX23">
     <cfRule type="colorScale" priority="1">
@@ -4111,6 +4136,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>